<commit_message>
Correction d'erreur dans la spreadsheet de wtf
</commit_message>
<xml_diff>
--- a/WtfSkin/BetSheet.xlsx
+++ b/WtfSkin/BetSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Vincent\Documents\Poly\H-18\H2018\WtfSkin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E52EF5-6FD6-4115-B3C9-BC24F38800EE}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD59E402-A12B-447D-AB4B-92E1F988EAC3}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{A8BCCCBA-D450-4E29-95A4-1310B68AE031}"/>
   </bookViews>
@@ -409,7 +409,7 @@
   <dimension ref="C2:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,18 +443,18 @@
       </c>
       <c r="D3">
         <f>E3</f>
-        <v>0.01</v>
+        <v>4.1999999999999997E-3</v>
       </c>
       <c r="E3">
-        <v>0.01</v>
+        <v>4.1999999999999997E-3</v>
       </c>
       <c r="F3">
         <f>E3*$J$3</f>
-        <v>1.5100000000000001E-2</v>
+        <v>6.3419999999999995E-3</v>
       </c>
       <c r="G3">
         <f>F3-D3</f>
-        <v>5.1000000000000004E-3</v>
+        <v>2.1419999999999998E-3</v>
       </c>
       <c r="I3">
         <v>2</v>
@@ -469,19 +469,19 @@
       </c>
       <c r="D4">
         <f>SUM($E$3:E4)</f>
-        <v>0.04</v>
+        <v>1.6799999999999999E-2</v>
       </c>
       <c r="E4">
         <f>E3*3</f>
-        <v>0.03</v>
+        <v>1.26E-2</v>
       </c>
       <c r="F4">
         <f t="shared" ref="F4:F11" si="0">E4*$J$3</f>
-        <v>4.53E-2</v>
+        <v>1.9026000000000001E-2</v>
       </c>
       <c r="G4">
         <f t="shared" ref="G4:G11" si="1">F4-D4</f>
-        <v>5.2999999999999992E-3</v>
+        <v>2.2260000000000023E-3</v>
       </c>
       <c r="I4" t="s">
         <v>7</v>
@@ -493,23 +493,23 @@
       </c>
       <c r="D5">
         <f>SUM($E$3:E5)</f>
-        <v>0.13</v>
+        <v>5.4599999999999996E-2</v>
       </c>
       <c r="E5">
         <f t="shared" ref="E5:E11" si="2">E4*3</f>
-        <v>0.09</v>
+        <v>3.78E-2</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>0.13589999999999999</v>
+        <v>5.7078000000000004E-2</v>
       </c>
       <c r="G5">
         <f t="shared" si="1"/>
-        <v>5.8999999999999886E-3</v>
+        <v>2.478000000000008E-3</v>
       </c>
       <c r="I5">
         <f>G3*I3</f>
-        <v>1.0200000000000001E-2</v>
+        <v>4.2839999999999996E-3</v>
       </c>
     </row>
     <row r="6" spans="3:10" x14ac:dyDescent="0.25">
@@ -518,19 +518,19 @@
       </c>
       <c r="D6">
         <f>SUM($E$3:E6)</f>
-        <v>0.4</v>
+        <v>0.16799999999999998</v>
       </c>
       <c r="E6">
         <f t="shared" si="2"/>
-        <v>0.27</v>
+        <v>0.1134</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>0.40770000000000001</v>
+        <v>0.171234</v>
       </c>
       <c r="G6">
         <f t="shared" si="1"/>
-        <v>7.6999999999999846E-3</v>
+        <v>3.2340000000000146E-3</v>
       </c>
       <c r="I6" t="s">
         <v>6</v>
@@ -542,23 +542,23 @@
       </c>
       <c r="D7">
         <f>SUM($E$3:E7)</f>
-        <v>1.21</v>
+        <v>0.50819999999999999</v>
       </c>
       <c r="E7">
         <f t="shared" si="2"/>
-        <v>0.81</v>
+        <v>0.3402</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>1.2231000000000001</v>
+        <v>0.51370199999999999</v>
       </c>
       <c r="G7">
         <f t="shared" si="1"/>
-        <v>1.3100000000000112E-2</v>
+        <v>5.5020000000000069E-3</v>
       </c>
       <c r="I7">
-        <f>(50/I5)/60</f>
-        <v>81.699346405228752</v>
+        <f>(10/I5)/60</f>
+        <v>38.904450669156553</v>
       </c>
       <c r="J7" t="s">
         <v>8</v>
@@ -570,23 +570,23 @@
       </c>
       <c r="D8">
         <f>SUM($E$3:E8)</f>
-        <v>3.64</v>
+        <v>1.5287999999999999</v>
       </c>
       <c r="E8">
         <f t="shared" si="2"/>
-        <v>2.4300000000000002</v>
+        <v>1.0206</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>3.6693000000000002</v>
+        <v>1.5411059999999999</v>
       </c>
       <c r="G8">
         <f t="shared" si="1"/>
-        <v>2.9300000000000104E-2</v>
+        <v>1.2305999999999928E-2</v>
       </c>
       <c r="I8">
         <f>I7/24</f>
-        <v>3.4041394335511979</v>
+        <v>1.621018777881523</v>
       </c>
       <c r="J8" t="s">
         <v>9</v>
@@ -598,19 +598,19 @@
       </c>
       <c r="D9">
         <f>SUM($E$3:E9)</f>
-        <v>10.930000000000001</v>
+        <v>4.5906000000000002</v>
       </c>
       <c r="E9">
         <f t="shared" si="2"/>
-        <v>7.2900000000000009</v>
+        <v>3.0617999999999999</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>11.007900000000001</v>
+        <v>4.6233179999999994</v>
       </c>
       <c r="G9">
         <f t="shared" si="1"/>
-        <v>7.7899999999999636E-2</v>
+        <v>3.2717999999999137E-2</v>
       </c>
     </row>
     <row r="10" spans="3:10" x14ac:dyDescent="0.25">
@@ -619,40 +619,40 @@
       </c>
       <c r="D10">
         <f>SUM($E$3:E10)</f>
-        <v>32.800000000000004</v>
+        <v>13.776</v>
       </c>
       <c r="E10">
         <f t="shared" si="2"/>
-        <v>21.870000000000005</v>
+        <v>9.1853999999999996</v>
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
-        <v>33.023700000000005</v>
+        <v>13.869954</v>
       </c>
       <c r="G10">
         <f t="shared" si="1"/>
-        <v>0.2237000000000009</v>
+        <v>9.3954000000000093E-2</v>
       </c>
     </row>
     <row r="11" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C11">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D11">
         <f>SUM($E$3:E11)</f>
-        <v>98.410000000000025</v>
+        <v>41.3322</v>
       </c>
       <c r="E11">
         <f t="shared" si="2"/>
-        <v>65.610000000000014</v>
+        <v>27.556199999999997</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
-        <v>99.071100000000015</v>
+        <v>41.609861999999993</v>
       </c>
       <c r="G11">
         <f t="shared" si="1"/>
-        <v>0.66109999999999047</v>
+        <v>0.2776619999999923</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajout de la formule pour calculer la mise optimale dans wtfSpredSheet
</commit_message>
<xml_diff>
--- a/WtfSkin/BetSheet.xlsx
+++ b/WtfSkin/BetSheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Vincent\Documents\Poly\H-18\H2018\WtfSkin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vince\Documents\Poly\H-18\gitEti\H2018\WtfSkin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD59E402-A12B-447D-AB4B-92E1F988EAC3}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53EDCD81-05F1-48F7-B523-8EC91C4F1550}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{A8BCCCBA-D450-4E29-95A4-1310B68AE031}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12216" xr2:uid="{A8BCCCBA-D450-4E29-95A4-1310B68AE031}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Mise</t>
   </si>
@@ -55,12 +55,30 @@
   </si>
   <si>
     <t>Jours</t>
+  </si>
+  <si>
+    <t>Formule:</t>
+  </si>
+  <si>
+    <t>(3^round - 1)/2</t>
+  </si>
+  <si>
+    <t>Round</t>
+  </si>
+  <si>
+    <t>Cash en banque</t>
+  </si>
+  <si>
+    <t>Mise optimale</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -90,8 +108,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -110,7 +129,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -406,18 +425,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CA5436F-1CDC-4E31-B725-2292178964AC}">
-  <dimension ref="C2:J11"/>
+  <dimension ref="C2:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="9" max="9" width="20.85546875" customWidth="1"/>
+    <col min="9" max="9" width="20.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:10" x14ac:dyDescent="0.3">
       <c r="D2" t="s">
         <v>3</v>
       </c>
@@ -437,24 +456,25 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
         <f>E3</f>
-        <v>4.1999999999999997E-3</v>
-      </c>
-      <c r="E3">
-        <v>4.1999999999999997E-3</v>
+        <v>1.34E-2</v>
+      </c>
+      <c r="E3" s="1">
+        <f>J15</f>
+        <v>1.34E-2</v>
       </c>
       <c r="F3">
         <f>E3*$J$3</f>
-        <v>6.3419999999999995E-3</v>
+        <v>2.0234000000000002E-2</v>
       </c>
       <c r="G3">
         <f>F3-D3</f>
-        <v>2.1419999999999998E-3</v>
+        <v>6.8340000000000015E-3</v>
       </c>
       <c r="I3">
         <v>2</v>
@@ -463,196 +483,227 @@
         <v>1.51</v>
       </c>
     </row>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C4">
         <v>2</v>
       </c>
       <c r="D4">
         <f>SUM($E$3:E4)</f>
-        <v>1.6799999999999999E-2</v>
+        <v>5.3600000000000002E-2</v>
       </c>
       <c r="E4">
         <f>E3*3</f>
-        <v>1.26E-2</v>
+        <v>4.02E-2</v>
       </c>
       <c r="F4">
         <f t="shared" ref="F4:F11" si="0">E4*$J$3</f>
-        <v>1.9026000000000001E-2</v>
+        <v>6.0701999999999999E-2</v>
       </c>
       <c r="G4">
         <f t="shared" ref="G4:G11" si="1">F4-D4</f>
-        <v>2.2260000000000023E-3</v>
+        <v>7.1019999999999972E-3</v>
       </c>
       <c r="I4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C5">
         <v>3</v>
       </c>
       <c r="D5">
         <f>SUM($E$3:E5)</f>
-        <v>5.4599999999999996E-2</v>
+        <v>0.17419999999999999</v>
       </c>
       <c r="E5">
         <f t="shared" ref="E5:E11" si="2">E4*3</f>
-        <v>3.78E-2</v>
+        <v>0.1206</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>5.7078000000000004E-2</v>
+        <v>0.18210599999999999</v>
       </c>
       <c r="G5">
         <f t="shared" si="1"/>
-        <v>2.478000000000008E-3</v>
+        <v>7.9059999999999964E-3</v>
       </c>
       <c r="I5">
         <f>G3*I3</f>
-        <v>4.2839999999999996E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+        <v>1.3668000000000003E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C6">
         <v>4</v>
       </c>
       <c r="D6">
         <f>SUM($E$3:E6)</f>
-        <v>0.16799999999999998</v>
+        <v>0.53600000000000003</v>
       </c>
       <c r="E6">
         <f t="shared" si="2"/>
-        <v>0.1134</v>
+        <v>0.36180000000000001</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>0.171234</v>
+        <v>0.54631799999999997</v>
       </c>
       <c r="G6">
         <f t="shared" si="1"/>
-        <v>3.2340000000000146E-3</v>
+        <v>1.0317999999999938E-2</v>
       </c>
       <c r="I6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C7">
         <v>5</v>
       </c>
       <c r="D7">
         <f>SUM($E$3:E7)</f>
-        <v>0.50819999999999999</v>
+        <v>1.6214</v>
       </c>
       <c r="E7">
         <f t="shared" si="2"/>
-        <v>0.3402</v>
+        <v>1.0853999999999999</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>0.51370199999999999</v>
+        <v>1.6389539999999998</v>
       </c>
       <c r="G7">
         <f t="shared" si="1"/>
-        <v>5.5020000000000069E-3</v>
+        <v>1.7553999999999848E-2</v>
       </c>
       <c r="I7">
         <f>(10/I5)/60</f>
-        <v>38.904450669156553</v>
+        <v>12.193932299287871</v>
       </c>
       <c r="J7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C8">
         <v>6</v>
       </c>
       <c r="D8">
         <f>SUM($E$3:E8)</f>
-        <v>1.5287999999999999</v>
+        <v>4.8775999999999993</v>
       </c>
       <c r="E8">
         <f t="shared" si="2"/>
-        <v>1.0206</v>
+        <v>3.2561999999999998</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>1.5411059999999999</v>
+        <v>4.9168620000000001</v>
       </c>
       <c r="G8">
         <f t="shared" si="1"/>
-        <v>1.2305999999999928E-2</v>
+        <v>3.9262000000000796E-2</v>
       </c>
       <c r="I8">
         <f>I7/24</f>
-        <v>1.621018777881523</v>
+        <v>0.50808051247032793</v>
       </c>
       <c r="J8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C9">
         <v>7</v>
       </c>
       <c r="D9">
         <f>SUM($E$3:E9)</f>
-        <v>4.5906000000000002</v>
+        <v>14.646199999999999</v>
       </c>
       <c r="E9">
         <f t="shared" si="2"/>
-        <v>3.0617999999999999</v>
+        <v>9.7685999999999993</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>4.6233179999999994</v>
+        <v>14.750585999999998</v>
       </c>
       <c r="G9">
         <f t="shared" si="1"/>
-        <v>3.2717999999999137E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
+        <v>0.10438599999999987</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C10">
         <v>8</v>
       </c>
       <c r="D10">
         <f>SUM($E$3:E10)</f>
-        <v>13.776</v>
+        <v>43.951999999999998</v>
       </c>
       <c r="E10">
         <f t="shared" si="2"/>
-        <v>9.1853999999999996</v>
+        <v>29.305799999999998</v>
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
-        <v>13.869954</v>
+        <v>44.251757999999995</v>
       </c>
       <c r="G10">
         <f t="shared" si="1"/>
-        <v>9.3954000000000093E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
+        <v>0.29975799999999708</v>
+      </c>
+    </row>
+    <row r="11" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C11">
         <v>9</v>
       </c>
       <c r="D11">
         <f>SUM($E$3:E11)</f>
-        <v>41.3322</v>
+        <v>131.86939999999998</v>
       </c>
       <c r="E11">
         <f t="shared" si="2"/>
-        <v>27.556199999999997</v>
+        <v>87.917399999999986</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
-        <v>41.609861999999993</v>
+        <v>132.75527399999999</v>
       </c>
       <c r="G11">
         <f t="shared" si="1"/>
-        <v>0.2776619999999923</v>
+        <v>0.88587400000000116</v>
+      </c>
+      <c r="I11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="I13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="I14" t="s">
+        <v>13</v>
+      </c>
+      <c r="J14">
+        <v>44.2</v>
+      </c>
+    </row>
+    <row r="15" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="I15" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15" s="1">
+        <f>_xlfn.FLOOR.MATH(J14/(((3^J13)-1)/2),0.0001)</f>
+        <v>1.34E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Amelioration de la spredsheet wtf
</commit_message>
<xml_diff>
--- a/WtfSkin/BetSheet.xlsx
+++ b/WtfSkin/BetSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vince\Documents\Poly\H-18\gitEti\H2018\WtfSkin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53EDCD81-05F1-48F7-B523-8EC91C4F1550}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED91C16-40C8-48CD-BB5F-AE3F745CDC33}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12216" xr2:uid="{A8BCCCBA-D450-4E29-95A4-1310B68AE031}"/>
   </bookViews>
@@ -45,9 +45,6 @@
     <t>RoundWin/minute</t>
   </si>
   <si>
-    <t>Temps pour faire 50$</t>
-  </si>
-  <si>
     <t>$ par minutes</t>
   </si>
   <si>
@@ -70,14 +67,18 @@
   </si>
   <si>
     <t>Mise optimale</t>
+  </si>
+  <si>
+    <t>Temps pour faire:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.0000"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -108,8 +109,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -428,7 +430,7 @@
   <dimension ref="C2:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -504,7 +506,7 @@
         <v>7.1019999999999972E-3</v>
       </c>
       <c r="I4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="3:10" x14ac:dyDescent="0.3">
@@ -553,7 +555,10 @@
         <v>1.0317999999999938E-2</v>
       </c>
       <c r="I6" t="s">
-        <v>6</v>
+        <v>14</v>
+      </c>
+      <c r="J6" s="2">
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="3:10" x14ac:dyDescent="0.3">
@@ -577,11 +582,11 @@
         <v>1.7553999999999848E-2</v>
       </c>
       <c r="I7">
-        <f>(10/I5)/60</f>
+        <f>(J6/I5)/60</f>
         <v>12.193932299287871</v>
       </c>
       <c r="J7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="3:10" x14ac:dyDescent="0.3">
@@ -609,7 +614,7 @@
         <v>0.50808051247032793</v>
       </c>
       <c r="J8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.3">
@@ -675,15 +680,15 @@
         <v>0.88587400000000116</v>
       </c>
       <c r="I11" t="s">
+        <v>9</v>
+      </c>
+      <c r="J11" t="s">
         <v>10</v>
-      </c>
-      <c r="J11" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="13" spans="3:10" x14ac:dyDescent="0.3">
       <c r="I13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J13">
         <v>8</v>
@@ -691,7 +696,7 @@
     </row>
     <row r="14" spans="3:10" x14ac:dyDescent="0.3">
       <c r="I14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J14">
         <v>44.2</v>
@@ -699,7 +704,7 @@
     </row>
     <row r="15" spans="3:10" x14ac:dyDescent="0.3">
       <c r="I15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J15" s="1">
         <f>_xlfn.FLOOR.MATH(J14/(((3^J13)-1)/2),0.0001)</f>

</xml_diff>